<commit_message>
Refactor ML estimation scripts and add correlation likelihood
Added new likelihood functions for correlated random effects (L_c_corr.m, L_c_int.m), modularized parameter vector conversion (from_theta.m, to_theta.m), and improved simulation and estimation workflow in est_ind.m. Removed obsolete code, updated file naming for clarity, and moved previous results to a dated results directory. Also added new simulation and data generation scripts, and updated summary statistics calculations to use the best parameter estimates across multiple initializations.
</commit_message>
<xml_diff>
--- a/Hours_worked.xlsx
+++ b/Hours_worked.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\CH_Research Dropbox\Assorted content\whales_own\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917A162F-B834-4907-95A4-F127CDDC61B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84521D2-9E7B-420D-9220-1ACFB3531AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="10008" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2880" yWindow="2292" windowWidth="30960" windowHeight="12168" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -514,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:M70"/>
+  <dimension ref="A2:M72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -578,7 +578,7 @@
       </c>
       <c r="J5" s="3">
         <f>SUM(B3:B167)</f>
-        <v>196.5</v>
+        <v>203.5</v>
       </c>
       <c r="L5" t="s">
         <v>14</v>
@@ -602,7 +602,7 @@
       </c>
       <c r="J6" s="5">
         <f>J5-M20</f>
-        <v>45.5</v>
+        <v>33.5</v>
       </c>
       <c r="L6" t="s">
         <v>15</v>
@@ -693,6 +693,9 @@
       <c r="L13" t="s">
         <v>26</v>
       </c>
+      <c r="M13">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -745,7 +748,7 @@
       </c>
       <c r="M20" s="7">
         <f xml:space="preserve"> SUM(M4:M19)</f>
-        <v>151</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -1130,6 +1133,22 @@
         <v>45866</v>
       </c>
       <c r="B70">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="1">
+        <v>45868</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
+        <v>45872</v>
+      </c>
+      <c r="B72">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor likelihood integration and update correlation estimation
Renamed and refactored captain-level likelihood integration functions for clarity (L_c_int → L_c_corr_int, captainLik_full → L_c_corr_int_v2). Updated all relevant calls to use new function names. Improved comments and fixed typos in likelihood and simulation scripts. Standardized save file names in est_correlation.m. Added and updated simulation and estimation code in sim_correlation.m and added sim_correlation.asv.
</commit_message>
<xml_diff>
--- a/Hours_worked.xlsx
+++ b/Hours_worked.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\CH_Research Dropbox\Assorted content\whales_own\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84521D2-9E7B-420D-9220-1ACFB3531AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79CF47DE-F171-439E-8FEC-5CAF951A9AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="2292" windowWidth="30960" windowHeight="12168" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="10008" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -516,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -578,7 +578,7 @@
       </c>
       <c r="J5" s="3">
         <f>SUM(B3:B167)</f>
-        <v>203.5</v>
+        <v>203</v>
       </c>
       <c r="L5" t="s">
         <v>14</v>
@@ -602,7 +602,7 @@
       </c>
       <c r="J6" s="5">
         <f>J5-M20</f>
-        <v>33.5</v>
+        <v>33</v>
       </c>
       <c r="L6" t="s">
         <v>15</v>
@@ -1149,7 +1149,7 @@
         <v>45872</v>
       </c>
       <c r="B72">
-        <v>6</v>
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix log-likelihood calculation and update simulation scripts
Corrects the log-likelihood computation in L_c_corr_int_v2.m by applying the log to the voyage likelihood. Updates comments and clarifies likelihood vs. log-likelihood in L_c_corr.m and L_v_corr_v2.m. Modifies sim_correlation.m to use new initial parameters and enables additional test cases. Adds Nelder-Mead minimization setup in est_ind.m. Also includes changes to Hours_worked.xlsx and renames sim_correlation_v2.m to sim_correlation_v2.asv with stored parameter values.
</commit_message>
<xml_diff>
--- a/Hours_worked.xlsx
+++ b/Hours_worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\CH_Research Dropbox\Assorted content\whales_own\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79CF47DE-F171-439E-8FEC-5CAF951A9AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4E17BB-F0E1-4CFD-8FFA-460D7DC5D7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="10008" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -514,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:M72"/>
+  <dimension ref="A2:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -578,7 +578,7 @@
       </c>
       <c r="J5" s="3">
         <f>SUM(B3:B167)</f>
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="L5" t="s">
         <v>14</v>
@@ -602,7 +602,7 @@
       </c>
       <c r="J6" s="5">
         <f>J5-M20</f>
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="L6" t="s">
         <v>15</v>
@@ -1150,6 +1150,11 @@
       </c>
       <c r="B72">
         <v>5.5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B73">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor estimation scripts and update simulation parameters
Refactored and cleaned up the estimation scripts for correlated models, including switching to newer likelihood function versions and streamlining optimization and result storage. Updated simulation parameters in sim_correlation.m (increased number of captains and max voyages), improved comments, and removed obsolete or backup files (.asv).
</commit_message>
<xml_diff>
--- a/Hours_worked.xlsx
+++ b/Hours_worked.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\CH_Research Dropbox\Assorted content\whales_own\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4E17BB-F0E1-4CFD-8FFA-460D7DC5D7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8317162D-3C3F-4E47-A340-D1178D99A528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="10008" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24192" yWindow="1152" windowWidth="30960" windowHeight="12168" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -514,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:M73"/>
+  <dimension ref="A2:M74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -578,7 +578,7 @@
       </c>
       <c r="J5" s="3">
         <f>SUM(B3:B167)</f>
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="L5" t="s">
         <v>14</v>
@@ -602,7 +602,7 @@
       </c>
       <c r="J6" s="5">
         <f>J5-M20</f>
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L6" t="s">
         <v>15</v>
@@ -1153,8 +1153,19 @@
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
+        <v>45873</v>
+      </c>
       <c r="B73">
         <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
+        <v>45874</v>
+      </c>
+      <c r="B74">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new ML estimation scripts and update optimization
Added est_correlation_v2.m and est_correlation_v2.asv for improved parameter estimation and post-estimation analysis. Updated est_correlation.m and sim_correlation.m to refine initial guess generation and noise perturbation strategies, and adjusted optimization settings. Deleted obsolete est_correlation.asv. Updated binary data and results files to reflect new estimation and simulation outputs.
</commit_message>
<xml_diff>
--- a/Hours_worked.xlsx
+++ b/Hours_worked.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\CH_Research Dropbox\Assorted content\whales_own\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8317162D-3C3F-4E47-A340-D1178D99A528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644977BA-A1B5-44FD-B7F0-5DC4FBD99369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24192" yWindow="1152" windowWidth="30960" windowHeight="12168" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="30960" windowHeight="12168" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -517,7 +517,7 @@
   <dimension ref="A2:M74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -578,7 +578,7 @@
       </c>
       <c r="J5" s="3">
         <f>SUM(B3:B167)</f>
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="L5" t="s">
         <v>14</v>
@@ -602,7 +602,7 @@
       </c>
       <c r="J6" s="5">
         <f>J5-M20</f>
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L6" t="s">
         <v>15</v>
@@ -1165,7 +1165,7 @@
         <v>45874</v>
       </c>
       <c r="B74">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add lambda parameter to simulation and update estimation
Introduced IE12_gen_data.m to include lambda as a production multiplier in simulation. Updated est_correlation_v3.m to handle lambda parameters, adjust summary statistics, and use the new simulation function. Removed temporary scripts and added new estimation results file.
</commit_message>
<xml_diff>
--- a/Hours_worked.xlsx
+++ b/Hours_worked.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\CH_Research Dropbox\Assorted content\whales_own\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644977BA-A1B5-44FD-B7F0-5DC4FBD99369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD33F720-46D3-407C-87F2-D3811F9E8E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="30960" windowHeight="12168" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -514,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:M74"/>
+  <dimension ref="A2:M75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -578,7 +578,7 @@
       </c>
       <c r="J5" s="3">
         <f>SUM(B3:B167)</f>
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="L5" t="s">
         <v>14</v>
@@ -602,7 +602,7 @@
       </c>
       <c r="J6" s="5">
         <f>J5-M20</f>
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="L6" t="s">
         <v>15</v>
@@ -1166,6 +1166,14 @@
       </c>
       <c r="B74">
         <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" s="1">
+        <v>45875</v>
+      </c>
+      <c r="B75">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor ML estimation scripts and add README
Renamed and reorganized ML estimation scripts for consistency (e.g., est_correlation_v3.m to est_corr_v3.m, sim_correlation.m to sim_corr.m, sim_independent.m to sim_ind.m). Added a comprehensive README.md to document the code structure and usage. Updated sim_corr.m with improved diagnostics and post-estimation analysis. Moved results files to a backup directory and deleted obsolete files. Minor updates to code logic and parameter initialization in sim_corr scripts.
</commit_message>
<xml_diff>
--- a/Hours_worked.xlsx
+++ b/Hours_worked.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\CH_Research Dropbox\Assorted content\whales_own\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD33F720-46D3-407C-87F2-D3811F9E8E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E378D613-7486-459F-9F7E-F0BD63F868C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="30960" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t xml:space="preserve">Work on: </t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>aug 10- aug16</t>
+  </si>
+  <si>
+    <t>aug17-aug23</t>
   </si>
 </sst>
 </file>
@@ -517,7 +520,7 @@
   <dimension ref="A2:M75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -578,7 +581,7 @@
       </c>
       <c r="J5" s="3">
         <f>SUM(B3:B167)</f>
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L5" t="s">
         <v>14</v>
@@ -602,7 +605,7 @@
       </c>
       <c r="J6" s="5">
         <f>J5-M20</f>
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="L6" t="s">
         <v>15</v>
@@ -707,11 +710,20 @@
       <c r="L14" t="s">
         <v>27</v>
       </c>
+      <c r="M14">
+        <v>19</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>45787</v>
       </c>
+      <c r="L15" t="s">
+        <v>28</v>
+      </c>
+      <c r="M15">
+        <v>19</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -748,7 +760,7 @@
       </c>
       <c r="M20" s="7">
         <f xml:space="preserve"> SUM(M4:M19)</f>
-        <v>170</v>
+        <v>208</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -1173,7 +1185,7 @@
         <v>45875</v>
       </c>
       <c r="B75">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove obsolete files and update output paths
Deleted unused figures, R scripts, and autosave files. Updated output and data paths in IE6.r, IE7.r, IE6_2.do, IE8.do, IE8_simulations.do, and IE9.do to improve organization and consistency. These changes help maintain a cleaner repository and ensure outputs are saved to the correct locations.
</commit_message>
<xml_diff>
--- a/Hours_worked.xlsx
+++ b/Hours_worked.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\CH_Research Dropbox\Assorted content\whales_own\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E378D613-7486-459F-9F7E-F0BD63F868C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B9E008-AED4-41D7-A37C-D403D88C0A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="30960" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6876" yWindow="3276" windowWidth="23400" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -517,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:M75"/>
+  <dimension ref="A2:M82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -581,7 +581,7 @@
       </c>
       <c r="J5" s="3">
         <f>SUM(B3:B167)</f>
-        <v>224</v>
+        <v>225.5</v>
       </c>
       <c r="L5" t="s">
         <v>14</v>
@@ -605,7 +605,7 @@
       </c>
       <c r="J6" s="5">
         <f>J5-M20</f>
-        <v>16</v>
+        <v>17.5</v>
       </c>
       <c r="L6" t="s">
         <v>15</v>
@@ -1186,6 +1186,47 @@
       </c>
       <c r="B75">
         <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
+        <v>45882</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
+        <v>45891</v>
+      </c>
+      <c r="B77">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="1">
+        <v>45892</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" s="1">
+        <v>45893</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" s="1">
+        <v>45894</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" s="1">
+        <v>45895</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
+        <v>45896</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update simulation parameters in sim_corr.m
Reduced the number of initialization points from 2 to 1 and increased the maximum iterations for optimization from 300 to 5000 in sim_corr.m. Updated Hours_worked.xlsx and sim_corr_unrestricted.mat with new data and results.
</commit_message>
<xml_diff>
--- a/Hours_worked.xlsx
+++ b/Hours_worked.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\CH_Research Dropbox\Assorted content\whales_own\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B9E008-AED4-41D7-A37C-D403D88C0A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8B768C-CBF2-475C-AB8D-1DBC06A4F483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6876" yWindow="3276" windowWidth="23400" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -520,7 +520,7 @@
   <dimension ref="A2:M82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -581,7 +581,7 @@
       </c>
       <c r="J5" s="3">
         <f>SUM(B3:B167)</f>
-        <v>225.5</v>
+        <v>232</v>
       </c>
       <c r="L5" t="s">
         <v>14</v>
@@ -605,7 +605,7 @@
       </c>
       <c r="J6" s="5">
         <f>J5-M20</f>
-        <v>17.5</v>
+        <v>24</v>
       </c>
       <c r="L6" t="s">
         <v>15</v>
@@ -1208,26 +1208,21 @@
       <c r="A78" s="1">
         <v>45892</v>
       </c>
+      <c r="B78">
+        <v>6.5</v>
+      </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="1">
-        <v>45893</v>
-      </c>
+      <c r="A79" s="1"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="1">
-        <v>45894</v>
-      </c>
+      <c r="A80" s="1"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" s="1">
-        <v>45895</v>
-      </c>
+      <c r="A81" s="1"/>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" s="1">
-        <v>45896</v>
-      </c>
+      <c r="A82" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>